<commit_message>
updated project name on documents
</commit_message>
<xml_diff>
--- a/documents/Project_Workplan.xlsx
+++ b/documents/Project_Workplan.xlsx
@@ -1,12 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Downloads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4D9B71A-C692-4DE4-B655-98D04A9D8C2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="28680" yWindow="660" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sayfa1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="khPrtRJk+pKXh+3pc3YL554CumXfyJ6uWkuVq5+2B5k="/>
@@ -16,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="32">
   <si>
     <t>WEEKS</t>
   </si>
@@ -109,68 +118,82 @@
   </si>
   <si>
     <t>Presentation</t>
+  </si>
+  <si>
+    <t>Multimodal-RAG-Based-Product-Recommendation-System</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode=";;;"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="11">
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
-    <font/>
+    <font>
+      <sz val="11"/>
+      <name val="Aptos Narrow"/>
+    </font>
     <font>
       <b/>
-      <sz val="20.0"/>
+      <sz val="20"/>
       <color rgb="FF555555"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
-      <sz val="8.0"/>
+      <sz val="8"/>
       <color rgb="FF666666"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
-      <sz val="15.0"/>
+      <sz val="15"/>
       <color rgb="FF555555"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color rgb="FF555555"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF555555"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF555555"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="162"/>
     </font>
   </fonts>
   <fills count="3">
@@ -178,7 +201,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -188,41 +211,59 @@
     </fill>
   </fills>
   <borders count="13">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left/>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
       <bottom style="medium">
         <color rgb="FFEEEEEE"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
       <bottom style="medium">
         <color rgb="FFEEEEEE"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
@@ -232,22 +273,29 @@
       <bottom style="medium">
         <color rgb="FFEEEEEE"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
+      <right/>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left/>
@@ -260,6 +308,7 @@
       <bottom style="medium">
         <color rgb="FFEEEEEE"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thick">
@@ -274,6 +323,7 @@
       <bottom style="medium">
         <color rgb="FFEEEEEE"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -286,6 +336,7 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -300,6 +351,7 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left/>
@@ -312,77 +364,84 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="20">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="3" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="5" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="6" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="7" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="8" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="9" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="10" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="11" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="12" fillId="2" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="11" fillId="2" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="10" fillId="2" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="11" fillId="2" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="12" fillId="2" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="11" fillId="2" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="11" fillId="2" fontId="1" numFmtId="164" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="11" fillId="2" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="11" fillId="2" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -572,452 +631,456 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B3:R1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="8.63"/>
-    <col customWidth="1" min="2" max="2" width="46.75"/>
-    <col customWidth="1" min="3" max="3" width="15.88"/>
-    <col customWidth="1" min="4" max="18" width="13.0"/>
-    <col customWidth="1" min="19" max="26" width="8.63"/>
+    <col min="1" max="1" width="6.42578125" customWidth="1"/>
+    <col min="2" max="2" width="46.7109375" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" customWidth="1"/>
+    <col min="4" max="18" width="13" customWidth="1"/>
+    <col min="19" max="26" width="8.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" ht="30.75" customHeight="1">
-      <c r="B3" s="1"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="3" t="s">
+    <row r="3" spans="2:18" ht="30.75" customHeight="1">
+      <c r="B3" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="16"/>
+      <c r="D3" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
-      <c r="N3" s="4"/>
-      <c r="O3" s="4"/>
-      <c r="P3" s="4"/>
-      <c r="Q3" s="4"/>
-      <c r="R3" s="5"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
+      <c r="L3" s="14"/>
+      <c r="M3" s="14"/>
+      <c r="N3" s="14"/>
+      <c r="O3" s="14"/>
+      <c r="P3" s="14"/>
+      <c r="Q3" s="14"/>
+      <c r="R3" s="15"/>
     </row>
-    <row r="4" ht="30.75" customHeight="1">
-      <c r="B4" s="6"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="8" t="s">
+    <row r="4" spans="2:18" ht="30.75" customHeight="1">
+      <c r="B4" s="17"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="E4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="F4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="9" t="s">
+      <c r="G4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H4" s="9" t="s">
+      <c r="H4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="9" t="s">
+      <c r="I4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J4" s="9" t="s">
+      <c r="J4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="K4" s="9" t="s">
+      <c r="K4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="L4" s="9" t="s">
+      <c r="L4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="M4" s="9" t="s">
+      <c r="M4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="N4" s="9" t="s">
+      <c r="N4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="O4" s="9" t="s">
+      <c r="O4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="P4" s="9" t="s">
+      <c r="P4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="Q4" s="9" t="s">
+      <c r="Q4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="R4" s="9" t="s">
+      <c r="R4" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" ht="22.5" customHeight="1">
-      <c r="B5" s="10" t="s">
+    <row r="5" spans="2:18" ht="22.5" customHeight="1">
+      <c r="B5" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="12">
-        <v>1.0</v>
-      </c>
-      <c r="E5" s="13">
-        <v>2.0</v>
-      </c>
-      <c r="F5" s="13">
-        <v>3.0</v>
-      </c>
-      <c r="G5" s="13">
-        <v>4.0</v>
-      </c>
-      <c r="H5" s="13">
-        <v>5.0</v>
-      </c>
-      <c r="I5" s="13">
-        <v>6.0</v>
-      </c>
-      <c r="J5" s="13">
-        <v>7.0</v>
-      </c>
-      <c r="K5" s="13">
-        <v>8.0</v>
-      </c>
-      <c r="L5" s="13">
-        <v>9.0</v>
-      </c>
-      <c r="M5" s="13">
-        <v>10.0</v>
-      </c>
-      <c r="N5" s="13">
-        <v>11.0</v>
-      </c>
-      <c r="O5" s="13">
-        <v>12.0</v>
-      </c>
-      <c r="P5" s="13">
-        <v>13.0</v>
-      </c>
-      <c r="Q5" s="13">
-        <v>14.0</v>
-      </c>
-      <c r="R5" s="13">
-        <v>15.0</v>
+      <c r="D5" s="5">
+        <v>1</v>
+      </c>
+      <c r="E5" s="6">
+        <v>2</v>
+      </c>
+      <c r="F5" s="6">
+        <v>3</v>
+      </c>
+      <c r="G5" s="6">
+        <v>4</v>
+      </c>
+      <c r="H5" s="6">
+        <v>5</v>
+      </c>
+      <c r="I5" s="6">
+        <v>6</v>
+      </c>
+      <c r="J5" s="6">
+        <v>7</v>
+      </c>
+      <c r="K5" s="6">
+        <v>8</v>
+      </c>
+      <c r="L5" s="6">
+        <v>9</v>
+      </c>
+      <c r="M5" s="6">
+        <v>10</v>
+      </c>
+      <c r="N5" s="6">
+        <v>11</v>
+      </c>
+      <c r="O5" s="6">
+        <v>12</v>
+      </c>
+      <c r="P5" s="6">
+        <v>13</v>
+      </c>
+      <c r="Q5" s="6">
+        <v>14</v>
+      </c>
+      <c r="R5" s="6">
+        <v>15</v>
       </c>
     </row>
-    <row r="6" ht="31.5" customHeight="1">
-      <c r="B6" s="14" t="s">
+    <row r="6" spans="2:18" ht="31.5" customHeight="1">
+      <c r="B6" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="16">
-        <v>1.0</v>
-      </c>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="17"/>
-      <c r="I6" s="17"/>
-      <c r="J6" s="17"/>
-      <c r="K6" s="17"/>
-      <c r="L6" s="17"/>
-      <c r="M6" s="17"/>
-      <c r="N6" s="17"/>
-      <c r="O6" s="17"/>
-      <c r="P6" s="17"/>
-      <c r="Q6" s="18"/>
-      <c r="R6" s="18"/>
+      <c r="D6" s="9">
+        <v>1</v>
+      </c>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="10"/>
+      <c r="M6" s="10"/>
+      <c r="N6" s="10"/>
+      <c r="O6" s="10"/>
+      <c r="P6" s="10"/>
+      <c r="Q6" s="11"/>
+      <c r="R6" s="11"/>
     </row>
-    <row r="7" ht="31.5" customHeight="1">
-      <c r="B7" s="14" t="s">
+    <row r="7" spans="2:18" ht="31.5" customHeight="1">
+      <c r="B7" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="16">
-        <v>1.0</v>
-      </c>
-      <c r="E7" s="17">
-        <v>2.0</v>
-      </c>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
-      <c r="H7" s="17"/>
-      <c r="I7" s="17"/>
-      <c r="J7" s="17"/>
-      <c r="K7" s="17"/>
-      <c r="L7" s="17"/>
-      <c r="M7" s="17"/>
-      <c r="N7" s="17"/>
-      <c r="O7" s="17"/>
-      <c r="P7" s="17"/>
-      <c r="Q7" s="18"/>
-      <c r="R7" s="18"/>
+      <c r="D7" s="9">
+        <v>1</v>
+      </c>
+      <c r="E7" s="10">
+        <v>2</v>
+      </c>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="10"/>
+      <c r="M7" s="10"/>
+      <c r="N7" s="10"/>
+      <c r="O7" s="10"/>
+      <c r="P7" s="10"/>
+      <c r="Q7" s="11"/>
+      <c r="R7" s="11"/>
     </row>
-    <row r="8" ht="31.5" customHeight="1">
-      <c r="B8" s="14" t="s">
+    <row r="8" spans="2:18" ht="31.5" customHeight="1">
+      <c r="B8" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="C8" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="16">
-        <v>1.0</v>
-      </c>
-      <c r="E8" s="17">
-        <v>2.0</v>
-      </c>
-      <c r="F8" s="17"/>
-      <c r="G8" s="17"/>
-      <c r="H8" s="17"/>
-      <c r="I8" s="17"/>
-      <c r="J8" s="17"/>
-      <c r="K8" s="17"/>
-      <c r="L8" s="17"/>
-      <c r="M8" s="17"/>
-      <c r="N8" s="17"/>
-      <c r="O8" s="17"/>
-      <c r="P8" s="17"/>
-      <c r="Q8" s="18"/>
-      <c r="R8" s="18"/>
+      <c r="D8" s="9">
+        <v>1</v>
+      </c>
+      <c r="E8" s="10">
+        <v>2</v>
+      </c>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="10"/>
+      <c r="M8" s="10"/>
+      <c r="N8" s="10"/>
+      <c r="O8" s="10"/>
+      <c r="P8" s="10"/>
+      <c r="Q8" s="11"/>
+      <c r="R8" s="11"/>
     </row>
-    <row r="9" ht="31.5" customHeight="1">
-      <c r="B9" s="14" t="s">
+    <row r="9" spans="2:18" ht="31.5" customHeight="1">
+      <c r="B9" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="C9" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="16"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="17">
-        <v>3.0</v>
-      </c>
-      <c r="G9" s="17"/>
-      <c r="H9" s="17"/>
-      <c r="I9" s="17"/>
-      <c r="J9" s="17"/>
-      <c r="K9" s="17"/>
-      <c r="L9" s="17"/>
-      <c r="M9" s="17"/>
-      <c r="N9" s="17"/>
-      <c r="O9" s="17"/>
-      <c r="P9" s="17"/>
-      <c r="Q9" s="18"/>
-      <c r="R9" s="18"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10">
+        <v>3</v>
+      </c>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="10"/>
+      <c r="M9" s="10"/>
+      <c r="N9" s="10"/>
+      <c r="O9" s="10"/>
+      <c r="P9" s="10"/>
+      <c r="Q9" s="11"/>
+      <c r="R9" s="11"/>
     </row>
-    <row r="10" ht="31.5" customHeight="1">
-      <c r="B10" s="14" t="s">
+    <row r="10" spans="2:18" ht="31.5" customHeight="1">
+      <c r="B10" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="19" t="s">
+      <c r="C10" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="16"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17">
-        <v>3.0</v>
-      </c>
-      <c r="G10" s="17">
-        <v>4.0</v>
-      </c>
-      <c r="H10" s="17"/>
-      <c r="I10" s="17"/>
-      <c r="J10" s="17"/>
-      <c r="K10" s="17"/>
-      <c r="L10" s="17"/>
-      <c r="M10" s="17"/>
-      <c r="N10" s="17"/>
-      <c r="O10" s="17"/>
-      <c r="P10" s="17"/>
-      <c r="Q10" s="18"/>
-      <c r="R10" s="18"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10">
+        <v>3</v>
+      </c>
+      <c r="G10" s="10">
+        <v>4</v>
+      </c>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="10"/>
+      <c r="M10" s="10"/>
+      <c r="N10" s="10"/>
+      <c r="O10" s="10"/>
+      <c r="P10" s="10"/>
+      <c r="Q10" s="11"/>
+      <c r="R10" s="11"/>
     </row>
-    <row r="11" ht="31.5" customHeight="1">
-      <c r="B11" s="14" t="s">
+    <row r="11" spans="2:18" ht="31.5" customHeight="1">
+      <c r="B11" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="20" t="s">
+      <c r="C11" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="9"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10">
+        <v>4</v>
+      </c>
+      <c r="H11" s="10">
+        <v>5</v>
+      </c>
+      <c r="I11" s="10">
+        <v>6</v>
+      </c>
+      <c r="J11" s="10"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="10"/>
+      <c r="M11" s="10"/>
+      <c r="N11" s="10"/>
+      <c r="O11" s="10"/>
+      <c r="P11" s="10"/>
+      <c r="Q11" s="11"/>
+      <c r="R11" s="11"/>
+    </row>
+    <row r="12" spans="2:18" ht="31.5" customHeight="1">
+      <c r="B12" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="16"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="17">
-        <v>4.0</v>
-      </c>
-      <c r="H11" s="17">
-        <v>5.0</v>
-      </c>
-      <c r="I11" s="17">
-        <v>6.0</v>
-      </c>
-      <c r="J11" s="17"/>
-      <c r="K11" s="17"/>
-      <c r="L11" s="17"/>
-      <c r="M11" s="17"/>
-      <c r="N11" s="17"/>
-      <c r="O11" s="17"/>
-      <c r="P11" s="17"/>
-      <c r="Q11" s="18"/>
-      <c r="R11" s="18"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10">
+        <v>6</v>
+      </c>
+      <c r="J12" s="10">
+        <v>7</v>
+      </c>
+      <c r="K12" s="10">
+        <v>8</v>
+      </c>
+      <c r="L12" s="10">
+        <v>9</v>
+      </c>
+      <c r="M12" s="10">
+        <v>10</v>
+      </c>
+      <c r="N12" s="10"/>
+      <c r="O12" s="10"/>
+      <c r="P12" s="10"/>
+      <c r="Q12" s="11"/>
+      <c r="R12" s="11"/>
     </row>
-    <row r="12" ht="31.5" customHeight="1">
-      <c r="B12" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="C12" s="20" t="s">
+    <row r="13" spans="2:18" ht="31.5" customHeight="1">
+      <c r="B13" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="16"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="17"/>
-      <c r="H12" s="17"/>
-      <c r="I12" s="17">
-        <v>6.0</v>
-      </c>
-      <c r="J12" s="17">
-        <v>7.0</v>
-      </c>
-      <c r="K12" s="17">
-        <v>8.0</v>
-      </c>
-      <c r="L12" s="17">
-        <v>9.0</v>
-      </c>
-      <c r="M12" s="17">
-        <v>10.0</v>
-      </c>
-      <c r="N12" s="17"/>
-      <c r="O12" s="17"/>
-      <c r="P12" s="17"/>
-      <c r="Q12" s="18"/>
-      <c r="R12" s="18"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="10"/>
+      <c r="M13" s="10">
+        <v>10</v>
+      </c>
+      <c r="N13" s="10">
+        <v>11</v>
+      </c>
+      <c r="O13" s="10"/>
+      <c r="P13" s="10"/>
+      <c r="Q13" s="11"/>
+      <c r="R13" s="11"/>
     </row>
-    <row r="13" ht="31.5" customHeight="1">
-      <c r="B13" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="C13" s="20" t="s">
+    <row r="14" spans="2:18" ht="31.5" customHeight="1">
+      <c r="B14" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="D13" s="16"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="17"/>
-      <c r="G13" s="17"/>
-      <c r="H13" s="17"/>
-      <c r="I13" s="17"/>
-      <c r="J13" s="17"/>
-      <c r="K13" s="17"/>
-      <c r="L13" s="17"/>
-      <c r="M13" s="17">
-        <v>10.0</v>
-      </c>
-      <c r="N13" s="17">
-        <v>11.0</v>
-      </c>
-      <c r="O13" s="17"/>
-      <c r="P13" s="17"/>
-      <c r="Q13" s="18"/>
-      <c r="R13" s="18"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="10"/>
+      <c r="M14" s="10">
+        <v>10</v>
+      </c>
+      <c r="N14" s="10">
+        <v>11</v>
+      </c>
+      <c r="O14" s="10">
+        <v>12</v>
+      </c>
+      <c r="P14" s="10">
+        <v>13</v>
+      </c>
+      <c r="Q14" s="11"/>
+      <c r="R14" s="11"/>
     </row>
-    <row r="14" ht="31.5" customHeight="1">
-      <c r="B14" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="C14" s="20" t="s">
+    <row r="15" spans="2:18" ht="31.5" customHeight="1">
+      <c r="B15" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="16"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="17"/>
-      <c r="H14" s="17"/>
-      <c r="I14" s="17"/>
-      <c r="J14" s="17"/>
-      <c r="K14" s="17"/>
-      <c r="L14" s="17"/>
-      <c r="M14" s="17">
-        <v>10.0</v>
-      </c>
-      <c r="N14" s="17">
-        <v>11.0</v>
-      </c>
-      <c r="O14" s="17">
-        <v>12.0</v>
-      </c>
-      <c r="P14" s="17">
-        <v>13.0</v>
-      </c>
-      <c r="Q14" s="18"/>
-      <c r="R14" s="18"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="10"/>
+      <c r="M15" s="10"/>
+      <c r="N15" s="10"/>
+      <c r="O15" s="10"/>
+      <c r="P15" s="10">
+        <v>13</v>
+      </c>
+      <c r="Q15" s="10">
+        <v>14</v>
+      </c>
+      <c r="R15" s="11">
+        <v>15</v>
+      </c>
     </row>
-    <row r="15" ht="31.5" customHeight="1">
-      <c r="B15" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="C15" s="20" t="s">
+    <row r="16" spans="2:18" ht="31.5" customHeight="1">
+      <c r="B16" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="D15" s="16"/>
-      <c r="E15" s="17"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="17"/>
-      <c r="H15" s="17"/>
-      <c r="I15" s="17"/>
-      <c r="J15" s="17"/>
-      <c r="K15" s="17"/>
-      <c r="L15" s="17"/>
-      <c r="M15" s="17"/>
-      <c r="N15" s="17"/>
-      <c r="O15" s="17"/>
-      <c r="P15" s="17">
-        <v>13.0</v>
-      </c>
-      <c r="Q15" s="17">
-        <v>14.0</v>
-      </c>
-      <c r="R15" s="18">
-        <v>15.0</v>
-      </c>
-    </row>
-    <row r="16" ht="31.5" customHeight="1">
-      <c r="B16" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="C16" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="D16" s="16"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="17"/>
-      <c r="H16" s="17"/>
-      <c r="I16" s="17"/>
-      <c r="J16" s="17"/>
-      <c r="K16" s="17"/>
-      <c r="L16" s="17"/>
-      <c r="M16" s="17"/>
-      <c r="N16" s="17"/>
-      <c r="O16" s="17"/>
-      <c r="P16" s="17"/>
-      <c r="Q16" s="18"/>
-      <c r="R16" s="18">
-        <v>15.0</v>
+      <c r="D16" s="9"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="10"/>
+      <c r="K16" s="10"/>
+      <c r="L16" s="10"/>
+      <c r="M16" s="10"/>
+      <c r="N16" s="10"/>
+      <c r="O16" s="10"/>
+      <c r="P16" s="10"/>
+      <c r="Q16" s="11"/>
+      <c r="R16" s="11">
+        <v>15</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1"/>
@@ -2014,8 +2077,6 @@
         <color rgb="FF24A7A4"/>
       </colorScale>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D6:R16">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -2024,8 +2085,6 @@
         <color rgb="FF0B769F"/>
       </colorScale>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D6:R16">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -2035,9 +2094,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>